<commit_message>
Update 1.5.13: Template fixes
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Шаблон для импорта Бригады.xlsx
+++ b/pkg/excels/templates/Шаблон для импорта Бригады.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\TGEM\tgem-backend\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D95A98-199D-4915-BE25-ECD884066718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Импорт" sheetId="1" r:id="rId1"/>
     <sheet name="Бригадиры" sheetId="2" r:id="rId2"/>
-    <sheet name="Объекты" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,25 +25,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <b/>
         <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>№ Бригады</t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
@@ -57,11 +55,11 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
@@ -73,11 +71,11 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
@@ -86,156 +84,158 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <b/>
         <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Компания</t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
     </r>
   </si>
   <si>
-    <r>
-      <t>Объект</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Имя Объекта</t>
-  </si>
-  <si>
-    <t>Тип Объекта</t>
-  </si>
-  <si>
     <t>Имя Бригадира</t>
   </si>
   <si>
-    <t>Комрон</t>
-  </si>
-  <si>
-    <t>Исмоил</t>
-  </si>
-  <si>
-    <t>ТП ИМПОРТ 2</t>
-  </si>
-  <si>
-    <t>ТП</t>
-  </si>
-  <si>
-    <t>ТП ИМПОРТ 1</t>
-  </si>
-  <si>
-    <t>СТВТ ИМПОРТ 2</t>
-  </si>
-  <si>
-    <t>СТВТ</t>
-  </si>
-  <si>
-    <t>СТВТ ИМПОРТ 1</t>
-  </si>
-  <si>
-    <t>СИП-ТЕСТ 2</t>
-  </si>
-  <si>
-    <t>СИП</t>
-  </si>
-  <si>
-    <t>СИП-ТЕСТ 1</t>
-  </si>
-  <si>
-    <t>Тест МЖД 2 ИМПОРТ</t>
-  </si>
-  <si>
-    <t>МЖД</t>
-  </si>
-  <si>
-    <t>Тест МЖД 1 ИМПОРТ</t>
-  </si>
-  <si>
-    <t>Тест Кл04КВ №3</t>
-  </si>
-  <si>
-    <t>КЛ 04 КВ</t>
-  </si>
-  <si>
-    <t>Тест Кл04КВ №2</t>
-  </si>
-  <si>
-    <t>Тест Кл04КВ №1</t>
-  </si>
-  <si>
-    <t>Тп тест 5</t>
-  </si>
-  <si>
-    <t>ТП ТЕСТ 2</t>
-  </si>
-  <si>
-    <t>ТП ТЕСТ 1</t>
-  </si>
-  <si>
-    <t>СТВТ ТЕСТ 4</t>
-  </si>
-  <si>
-    <t>СТВТ ТЕСТ 2</t>
-  </si>
-  <si>
-    <t>СТВТ ТЕСТ 1</t>
-  </si>
-  <si>
-    <t>СИП НОВЫЙ ТЕСТ 2</t>
-  </si>
-  <si>
-    <t>СИП ТЕСТ 3</t>
-  </si>
-  <si>
-    <t>СИП ТЕСТ 2</t>
-  </si>
-  <si>
-    <t>Тест МЖД Новая страница</t>
-  </si>
-  <si>
-    <t>Тест МЖД 3</t>
-  </si>
-  <si>
-    <t>Тест МЖД 2</t>
-  </si>
-  <si>
-    <t>Тест на создание 2</t>
-  </si>
-  <si>
-    <t>Тест на создание 1</t>
-  </si>
-  <si>
-    <t>305/4</t>
+    <t>Гуломов Мухаммадисо</t>
+  </si>
+  <si>
+    <t>Отахонов Анвар</t>
+  </si>
+  <si>
+    <t>Бобочонов Хуршед</t>
+  </si>
+  <si>
+    <t>Хабибов Рамзулло</t>
+  </si>
+  <si>
+    <t>Точидинзода Дилшод</t>
+  </si>
+  <si>
+    <t>Назаров Далер</t>
+  </si>
+  <si>
+    <t>Рачабов Худойдод</t>
+  </si>
+  <si>
+    <t>Ашуров Нодир</t>
+  </si>
+  <si>
+    <t>Хонбоев Навруз</t>
+  </si>
+  <si>
+    <t>Достонов Муродулохон</t>
+  </si>
+  <si>
+    <t>Камолов Чахонгир</t>
+  </si>
+  <si>
+    <t>Ахунов Абдували</t>
+  </si>
+  <si>
+    <t>Меликбоев Ашурбой</t>
+  </si>
+  <si>
+    <t>Файзов Алишер</t>
+  </si>
+  <si>
+    <t>Шарифзода Шахбон</t>
+  </si>
+  <si>
+    <t>Хочаев Амрохон</t>
+  </si>
+  <si>
+    <t>Ватанов Мубин</t>
+  </si>
+  <si>
+    <t>Беков Чамшед</t>
+  </si>
+  <si>
+    <t>Иброхимов Зайнуддин</t>
+  </si>
+  <si>
+    <t>Сафаров Чавохир</t>
+  </si>
+  <si>
+    <t>Абдусамадов Хадиятулло</t>
+  </si>
+  <si>
+    <t>Нормурадов Рашид</t>
+  </si>
+  <si>
+    <t>Муродов Чамшед</t>
+  </si>
+  <si>
+    <t>Фирузчони Чурахон</t>
+  </si>
+  <si>
+    <t>Рахматшоев Рахматулло</t>
+  </si>
+  <si>
+    <t>Шарифов Бадриддин</t>
+  </si>
+  <si>
+    <t>Сатторов Сухроб</t>
+  </si>
+  <si>
+    <t>Тоиров Ёкуб</t>
+  </si>
+  <si>
+    <t>Мирзоев Карим</t>
+  </si>
+  <si>
+    <t>Сайдалиев Аюбчон</t>
+  </si>
+  <si>
+    <t>Эмомалии Рахмонали</t>
+  </si>
+  <si>
+    <t>Холов Ёрахмад</t>
+  </si>
+  <si>
+    <t>Алиев Рачабали</t>
+  </si>
+  <si>
+    <t>Сухроби Талби</t>
+  </si>
+  <si>
+    <t>Саторов Хочимурод</t>
+  </si>
+  <si>
+    <t>Газабов Хабибулло</t>
+  </si>
+  <si>
+    <t>Саидов Саймахмуд</t>
+  </si>
+  <si>
+    <t>Хучаков Давлат</t>
+  </si>
+  <si>
+    <t>Зарипов Шамсиддин</t>
+  </si>
+  <si>
+    <t>Гафоров Сайфулло.</t>
+  </si>
+  <si>
+    <t>Файзов Ахлиддин</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,7 +244,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -252,7 +252,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -260,7 +260,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -268,7 +268,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -297,14 +297,14 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -317,7 +317,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -578,11 +578,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,27 +606,25 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{C59A472F-E5DD-4656-879C-598775FE6A4B}"/>
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{89AE8123-557A-48E2-87BA-3A0461F77877}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Бригадиры!$A$2:$A$116</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B297</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{019A999F-8215-45A0-A9D0-E35AD7430825}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Объекты!$A$2:$A$122</xm:f>
+            <xm:f>#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
@@ -637,274 +635,226 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097094F9-7E6F-44E4-B859-0524084CD09F}">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="true" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col bestFit="true" customWidth="true" max="1" min="1" width="15.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="6">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82AF30F3-BB4D-46EB-8BB6-A0A987AA3E31}">
-  <dimension ref="A1:B28"/>
-  <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="7">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="9">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="12">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="15">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="18">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="21">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
         <v>33</v>
       </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
         <v>35</v>
       </c>
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
         <v>36</v>
       </c>
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
         <v>37</v>
       </c>
-      <c r="B25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
         <v>38</v>
       </c>
-      <c r="B26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
         <v>39</v>
       </c>
-      <c r="B27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
         <v>40</v>
       </c>
-      <c r="B28" t="s">
-        <v>11</v>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>